<commit_message>
refactor: internationalize codebase to English
- Convert all Python docstrings and comments to English
- Translate CSV test data to English (headers and content)
- Update all console output messages to English
- Translate PPT generator style names and messages to English
- Keep README.md in Chinese as per project requirement

This change improves international collaboration while maintaining
Chinese documentation for local users.

Files modified: 13 (+309, -382 lines)
</commit_message>
<xml_diff>
--- a/data/input/sample.xlsx
+++ b/data/input/sample.xlsx
@@ -16,61 +16,61 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
-    <t>姓名</t>
-  </si>
-  <si>
-    <t>年龄</t>
-  </si>
-  <si>
-    <t>部门</t>
-  </si>
-  <si>
-    <t>工资</t>
-  </si>
-  <si>
-    <t>绩效得分</t>
-  </si>
-  <si>
-    <t>张三</t>
-  </si>
-  <si>
-    <t>李四</t>
-  </si>
-  <si>
-    <t>王五</t>
-  </si>
-  <si>
-    <t>赵六</t>
-  </si>
-  <si>
-    <t>钱七</t>
-  </si>
-  <si>
-    <t>孙八</t>
-  </si>
-  <si>
-    <t>周九</t>
-  </si>
-  <si>
-    <t>吴十</t>
-  </si>
-  <si>
-    <t>郑十一</t>
-  </si>
-  <si>
-    <t>王十二</t>
-  </si>
-  <si>
-    <t>技术部</t>
-  </si>
-  <si>
-    <t>销售部</t>
-  </si>
-  <si>
-    <t>市场部</t>
-  </si>
-  <si>
-    <t>人事部</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Performance Score</t>
+  </si>
+  <si>
+    <t>Zhang San</t>
+  </si>
+  <si>
+    <t>Li Si</t>
+  </si>
+  <si>
+    <t>Wang Wu</t>
+  </si>
+  <si>
+    <t>Zhao Liu</t>
+  </si>
+  <si>
+    <t>Qian Qi</t>
+  </si>
+  <si>
+    <t>Sun Ba</t>
+  </si>
+  <si>
+    <t>Zhou Jiu</t>
+  </si>
+  <si>
+    <t>Wu Shi</t>
+  </si>
+  <si>
+    <t>Zheng Shiyi</t>
+  </si>
+  <si>
+    <t>Wang Shier</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>HR</t>
   </si>
 </sst>
 </file>

</xml_diff>